<commit_message>
refined parts of the document
Signed-off-by: Dina Benayad-Cherif <dina.benayad.cherif@gmail.com>
</commit_message>
<xml_diff>
--- a/ParallelizationAnalysis.xlsx
+++ b/ParallelizationAnalysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>Cleveland</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Tweets to Stream And Analyze</t>
+  </si>
+  <si>
+    <t>Cleveland (seconds)</t>
+  </si>
+  <si>
+    <t>Georgia (seconds)</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1068,7 @@
   <dimension ref="B3:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1098,7 +1104,7 @@
     </row>
     <row r="5" spans="2:7">
       <c r="C5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>15.898999999999999</v>
@@ -1115,7 +1121,7 @@
     </row>
     <row r="6" spans="2:7">
       <c r="C6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>9.3490000000000002</v>
@@ -1159,7 +1165,7 @@
     </row>
     <row r="10" spans="2:7">
       <c r="C10" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>18.664999999999999</v>
@@ -1176,7 +1182,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="C11" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>7.5359999999999996</v>

</xml_diff>